<commit_message>
adding new populations splits
</commit_message>
<xml_diff>
--- a/dict_master.xlsx
+++ b/dict_master.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sghedu-my.sharepoint.com/personal/rr109174_student_sgh_waw_pl/Documents/WarsawEconometricChallenge/WarsawEconometricChallenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC10488069986F345BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C72497-BA28-4AAA-8250-304B5FA60784}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="11_F25DC773A252ABDACC10488069986F345BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDB83864-5DD7-4522-8720-897886170463}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2175" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2175" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="241">
   <si>
     <t>municipality_code</t>
   </si>
@@ -509,9 +510,6 @@
     <t>population per a generally accessible pharmacy</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>average usable area of the apartment per person</t>
   </si>
   <si>
@@ -756,6 +754,12 @@
   </si>
   <si>
     <t>glosy_NIEM</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
   </si>
 </sst>
 </file>
@@ -1082,28 +1086,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="85.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.26953125" customWidth="1"/>
+    <col min="4" max="4" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
         <v>200</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1111,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1122,16 +1127,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
         <v>196</v>
       </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1142,7 +1147,7 @@
         <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -1156,7 +1161,7 @@
         <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -1170,7 +1175,7 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -1184,7 +1189,7 @@
         <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1198,7 +1203,7 @@
         <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1212,7 +1217,7 @@
         <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -1227,7 +1232,7 @@
         <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1242,7 +1247,7 @@
         <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1257,7 +1262,7 @@
         <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -1272,7 +1277,7 @@
         <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1287,7 +1292,7 @@
         <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -1302,7 +1307,7 @@
         <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -1316,7 +1321,7 @@
         <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1330,7 +1335,7 @@
         <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -1344,7 +1349,7 @@
         <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -1358,7 +1363,7 @@
         <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
@@ -1372,7 +1377,7 @@
         <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -1386,7 +1391,7 @@
         <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1400,7 +1405,7 @@
         <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -1414,7 +1419,7 @@
         <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
@@ -1428,7 +1433,7 @@
         <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -1442,7 +1447,7 @@
         <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -1456,7 +1461,7 @@
         <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D26" t="s">
         <v>23</v>
@@ -1470,7 +1475,7 @@
         <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" t="s">
         <v>24</v>
@@ -1484,7 +1489,7 @@
         <v>122</v>
       </c>
       <c r="C28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
@@ -1498,7 +1503,7 @@
         <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
@@ -1512,7 +1517,7 @@
         <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -1526,7 +1531,7 @@
         <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -1540,7 +1545,7 @@
         <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -1554,7 +1559,7 @@
         <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
@@ -1568,7 +1573,7 @@
         <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
         <v>31</v>
@@ -1582,7 +1587,7 @@
         <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -1596,7 +1601,7 @@
         <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D36" t="s">
         <v>33</v>
@@ -1610,7 +1615,7 @@
         <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D37" t="s">
         <v>34</v>
@@ -1624,7 +1629,7 @@
         <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
@@ -1638,7 +1643,7 @@
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s">
         <v>36</v>
@@ -1652,7 +1657,7 @@
         <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D40" t="s">
         <v>37</v>
@@ -1666,7 +1671,7 @@
         <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
@@ -1680,7 +1685,7 @@
         <v>136</v>
       </c>
       <c r="C42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -1694,7 +1699,7 @@
         <v>137</v>
       </c>
       <c r="C43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D43" t="s">
         <v>40</v>
@@ -1708,7 +1713,7 @@
         <v>138</v>
       </c>
       <c r="C44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D44" t="s">
         <v>41</v>
@@ -1722,7 +1727,7 @@
         <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
@@ -1736,7 +1741,7 @@
         <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s">
         <v>43</v>
@@ -1750,7 +1755,7 @@
         <v>141</v>
       </c>
       <c r="C47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D47" t="s">
         <v>44</v>
@@ -1764,7 +1769,7 @@
         <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D48" t="s">
         <v>45</v>
@@ -1778,7 +1783,7 @@
         <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D49" t="s">
         <v>46</v>
@@ -1792,7 +1797,7 @@
         <v>144</v>
       </c>
       <c r="C50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D50" t="s">
         <v>47</v>
@@ -1806,7 +1811,7 @@
         <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D51" t="s">
         <v>48</v>
@@ -1820,7 +1825,7 @@
         <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D52" t="s">
         <v>49</v>
@@ -1834,7 +1839,7 @@
         <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s">
         <v>50</v>
@@ -1848,7 +1853,7 @@
         <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D54" t="s">
         <v>51</v>
@@ -1862,7 +1867,7 @@
         <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D55" t="s">
         <v>52</v>
@@ -1876,7 +1881,7 @@
         <v>150</v>
       </c>
       <c r="C56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D56" t="s">
         <v>53</v>
@@ -1890,7 +1895,7 @@
         <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D57" t="s">
         <v>54</v>
@@ -1904,7 +1909,7 @@
         <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D58" t="s">
         <v>55</v>
@@ -1918,7 +1923,7 @@
         <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D59" t="s">
         <v>56</v>
@@ -1932,7 +1937,7 @@
         <v>154</v>
       </c>
       <c r="C60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" t="s">
         <v>57</v>
@@ -1946,7 +1951,7 @@
         <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D61" t="s">
         <v>58</v>
@@ -1960,7 +1965,7 @@
         <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D62" t="s">
         <v>60</v>
@@ -1971,10 +1976,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D63" t="s">
         <v>61</v>
@@ -1985,10 +1990,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
@@ -1999,10 +2004,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -2013,10 +2018,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
         <v>64</v>
@@ -2027,10 +2032,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D67" t="s">
         <v>65</v>
@@ -2041,10 +2046,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D68" t="s">
         <v>66</v>
@@ -2055,10 +2060,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D69" t="s">
         <v>67</v>
@@ -2069,10 +2074,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" t="s">
         <v>68</v>
@@ -2083,10 +2088,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D71" t="s">
         <v>69</v>
@@ -2097,10 +2102,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D72" t="s">
         <v>70</v>
@@ -2111,10 +2116,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D73" t="s">
         <v>71</v>
@@ -2125,10 +2130,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D74" t="s">
         <v>72</v>
@@ -2139,10 +2144,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D75" t="s">
         <v>73</v>
@@ -2153,10 +2158,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D76" t="s">
         <v>74</v>
@@ -2167,10 +2172,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D77" t="s">
         <v>75</v>
@@ -2181,10 +2186,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D78" t="s">
         <v>76</v>
@@ -2195,10 +2200,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D79" t="s">
         <v>77</v>
@@ -2209,10 +2214,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D80" t="s">
         <v>78</v>
@@ -2223,10 +2228,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D81" t="s">
         <v>79</v>
@@ -2237,10 +2242,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D82" t="s">
         <v>80</v>
@@ -2251,10 +2256,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D83" t="s">
         <v>81</v>
@@ -2265,10 +2270,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D84" t="s">
         <v>82</v>
@@ -2279,10 +2284,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D85" t="s">
         <v>83</v>
@@ -2293,10 +2298,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D86" t="s">
         <v>84</v>
@@ -2307,10 +2312,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D87" t="s">
         <v>85</v>
@@ -2321,10 +2326,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C88" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -2335,10 +2340,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D89" t="s">
         <v>87</v>
@@ -2349,10 +2354,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D90" t="s">
         <v>88</v>
@@ -2363,10 +2368,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D91" t="s">
         <v>89</v>
@@ -2377,10 +2382,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D92" t="s">
         <v>90</v>
@@ -2391,10 +2396,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D93" t="s">
         <v>91</v>
@@ -2405,10 +2410,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D94" t="s">
         <v>92</v>
@@ -2419,10 +2424,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D95" t="s">
         <v>93</v>
@@ -2433,10 +2438,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C96" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D96" t="s">
         <v>94</v>
@@ -2447,10 +2452,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C97" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D97" t="s">
         <v>95</v>
@@ -2461,10 +2466,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C98" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D98" t="s">
         <v>96</v>
@@ -2475,10 +2480,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D99" t="s">
         <v>97</v>
@@ -2486,27 +2491,27 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B100" t="s">
         <v>59</v>
       </c>
       <c r="C100" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D100" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
         <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D101" t="str">
         <f>LOWER(A101)</f>
@@ -2515,28 +2520,28 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B102" t="s">
         <v>59</v>
       </c>
       <c r="C102" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" ref="D102:D119" si="0">LOWER(A102)</f>
+        <f t="shared" ref="D102:D104" si="0">LOWER(A102)</f>
         <v>powiat</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B103" t="s">
         <v>59</v>
       </c>
       <c r="C103" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
@@ -2545,13 +2550,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B104" t="s">
         <v>59</v>
       </c>
       <c r="C104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
@@ -2561,216 +2566,287 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B105" t="s">
         <v>59</v>
       </c>
       <c r="C105" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105" t="s">
         <v>224</v>
-      </c>
-      <c r="D105" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B106" t="s">
         <v>59</v>
       </c>
       <c r="C106" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D106" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B107" t="s">
         <v>59</v>
       </c>
       <c r="C107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
         <v>59</v>
       </c>
       <c r="C108" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B109" t="s">
         <v>59</v>
       </c>
       <c r="C109" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D109" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B110" t="s">
         <v>59</v>
       </c>
       <c r="C110" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D110" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B111" t="s">
         <v>59</v>
       </c>
       <c r="C111" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D111" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B112" t="s">
         <v>59</v>
       </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D112" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B113" t="s">
         <v>59</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B114" t="s">
         <v>59</v>
       </c>
       <c r="C114" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D114" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B115" t="s">
         <v>59</v>
       </c>
       <c r="C115" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D115" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B116" t="s">
         <v>59</v>
       </c>
       <c r="C116" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D116" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B117" t="s">
         <v>59</v>
       </c>
       <c r="C117" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D117" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B118" t="s">
         <v>59</v>
       </c>
       <c r="C118" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D118" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B119" t="s">
         <v>59</v>
       </c>
       <c r="C119" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D119" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49745861-A84E-4248-9F1B-80C7799657BC}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>